<commit_message>
Segregating Currrent from Past
</commit_message>
<xml_diff>
--- a/Fix/fix cur. 23.xlsx
+++ b/Fix/fix cur. 23.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="51">
   <si>
     <t>amt</t>
   </si>
@@ -164,12 +164,6 @@
   </si>
   <si>
     <t>50300091974896</t>
-  </si>
-  <si>
-    <t>12+25</t>
-  </si>
-  <si>
-    <t>8911584817</t>
   </si>
   <si>
     <t>12 EOM</t>
@@ -806,10 +800,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:U113"/>
+  <dimension ref="A1:U112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34:XFD34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1327,7 +1321,7 @@
         <v>9.6</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D14" s="8" t="s">
         <v>6</v>
@@ -2087,34 +2081,16 @@
       <c r="U33" s="4"/>
     </row>
     <row r="34" spans="1:21" ht="12.75" customHeight="1">
-      <c r="A34" s="3">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="B34" s="3">
-        <v>9.0299999999999994</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>42</v>
-      </c>
+      <c r="A34" s="3"/>
+      <c r="B34" s="7"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
       <c r="F34" s="3"/>
-      <c r="G34" s="5">
-        <v>42135</v>
-      </c>
-      <c r="H34" s="5">
-        <v>42526</v>
-      </c>
-      <c r="I34" s="16">
-        <v>1687</v>
-      </c>
-      <c r="J34" s="6" t="s">
-        <v>51</v>
-      </c>
+      <c r="G34" s="3"/>
+      <c r="H34" s="3"/>
+      <c r="I34" s="7"/>
+      <c r="J34" s="3"/>
       <c r="K34" s="3"/>
       <c r="L34" s="4"/>
       <c r="M34" s="4"/>
@@ -2133,7 +2109,10 @@
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
       <c r="E35" s="3"/>
-      <c r="F35" s="3"/>
+      <c r="F35" s="3">
+        <f>SUM(A29:A33)</f>
+        <v>17.200000000000003</v>
+      </c>
       <c r="G35" s="3"/>
       <c r="H35" s="3"/>
       <c r="I35" s="7"/>
@@ -2156,10 +2135,7 @@
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
       <c r="E36" s="3"/>
-      <c r="F36" s="3">
-        <f>SUM(A29:A34)</f>
-        <v>19.400000000000002</v>
-      </c>
+      <c r="F36" s="3"/>
       <c r="G36" s="3"/>
       <c r="H36" s="3"/>
       <c r="I36" s="7"/>
@@ -2182,11 +2158,15 @@
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
       <c r="E37" s="3"/>
-      <c r="F37" s="3"/>
       <c r="G37" s="3"/>
       <c r="H37" s="3"/>
-      <c r="I37" s="7"/>
-      <c r="J37" s="3"/>
+      <c r="I37" s="7">
+        <f>SUM(I3:I33)</f>
+        <v>99462</v>
+      </c>
+      <c r="J37" s="3" t="s">
+        <v>3</v>
+      </c>
       <c r="K37" s="3"/>
       <c r="L37" s="4"/>
       <c r="M37" s="4"/>
@@ -2202,17 +2182,17 @@
     <row r="38" spans="1:21" ht="12.75" customHeight="1">
       <c r="A38" s="3"/>
       <c r="B38" s="7"/>
-      <c r="C38" s="3"/>
-      <c r="D38" s="3"/>
-      <c r="E38" s="3"/>
-      <c r="G38" s="3"/>
-      <c r="H38" s="3"/>
+      <c r="C38" s="7"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
+      <c r="G38" s="4"/>
+      <c r="H38" s="4"/>
       <c r="I38" s="7">
-        <f>SUM(I3:I34)</f>
-        <v>101149</v>
+        <v>18095</v>
       </c>
       <c r="J38" s="3" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="K38" s="3"/>
       <c r="L38" s="4"/>
@@ -2228,19 +2208,14 @@
     </row>
     <row r="39" spans="1:21" ht="12.75" customHeight="1">
       <c r="A39" s="3"/>
-      <c r="B39" s="7"/>
-      <c r="C39" s="7"/>
+      <c r="C39" s="4"/>
       <c r="D39" s="4"/>
       <c r="E39" s="4"/>
       <c r="F39" s="4"/>
       <c r="G39" s="4"/>
       <c r="H39" s="4"/>
-      <c r="I39" s="7">
-        <v>18095</v>
-      </c>
-      <c r="J39" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="I39" s="17"/>
+      <c r="J39" s="3"/>
       <c r="K39" s="3"/>
       <c r="L39" s="4"/>
       <c r="M39" s="4"/>
@@ -2254,14 +2229,22 @@
       <c r="U39" s="4"/>
     </row>
     <row r="40" spans="1:21" ht="12.75" customHeight="1">
-      <c r="A40" s="3"/>
+      <c r="A40" s="48">
+        <v>42138</v>
+      </c>
+      <c r="B40" s="7"/>
       <c r="C40" s="4"/>
       <c r="D40" s="4"/>
       <c r="E40" s="4"/>
-      <c r="F40" s="4"/>
-      <c r="G40" s="4"/>
+      <c r="F40" s="1">
+        <f>SUM(F3:F35)</f>
+        <v>125.4</v>
+      </c>
       <c r="H40" s="4"/>
-      <c r="I40" s="17"/>
+      <c r="I40" s="14">
+        <f>I37+I38</f>
+        <v>117557</v>
+      </c>
       <c r="J40" s="3"/>
       <c r="K40" s="3"/>
       <c r="L40" s="4"/>
@@ -2276,22 +2259,12 @@
       <c r="U40" s="4"/>
     </row>
     <row r="41" spans="1:21" ht="12.75" customHeight="1">
-      <c r="A41" s="48">
-        <v>42138</v>
-      </c>
-      <c r="B41" s="7"/>
-      <c r="C41" s="4"/>
-      <c r="D41" s="4"/>
-      <c r="E41" s="4"/>
-      <c r="F41" s="1">
-        <f>SUM(F3:F36)</f>
-        <v>127.60000000000001</v>
-      </c>
+      <c r="A41" s="4"/>
+      <c r="B41" s="4"/>
+      <c r="C41" s="25"/>
+      <c r="D41" s="12"/>
       <c r="H41" s="4"/>
-      <c r="I41" s="14">
-        <f>I38+I39</f>
-        <v>119244</v>
-      </c>
+      <c r="I41" s="4"/>
       <c r="J41" s="3"/>
       <c r="K41" s="3"/>
       <c r="L41" s="4"/>
@@ -2308,8 +2281,8 @@
     <row r="42" spans="1:21" ht="12.75" customHeight="1">
       <c r="A42" s="4"/>
       <c r="B42" s="4"/>
-      <c r="C42" s="25"/>
-      <c r="D42" s="12"/>
+      <c r="C42" s="11"/>
+      <c r="E42" s="4"/>
       <c r="H42" s="4"/>
       <c r="I42" s="4"/>
       <c r="J42" s="3"/>
@@ -2328,11 +2301,14 @@
     <row r="43" spans="1:21" ht="12.75" customHeight="1">
       <c r="A43" s="4"/>
       <c r="B43" s="4"/>
-      <c r="C43" s="11"/>
+      <c r="C43" s="4"/>
+      <c r="D43" s="4"/>
       <c r="E43" s="4"/>
-      <c r="H43" s="4"/>
+      <c r="F43" s="4"/>
+      <c r="G43" s="4"/>
+      <c r="H43" s="7"/>
       <c r="I43" s="4"/>
-      <c r="J43" s="3"/>
+      <c r="J43" s="36"/>
       <c r="K43" s="3"/>
       <c r="L43" s="4"/>
       <c r="M43" s="4"/>
@@ -2346,14 +2322,22 @@
       <c r="U43" s="4"/>
     </row>
     <row r="44" spans="1:21" ht="12.75" customHeight="1">
-      <c r="A44" s="4"/>
-      <c r="B44" s="4"/>
-      <c r="C44" s="4"/>
-      <c r="D44" s="4"/>
-      <c r="E44" s="4"/>
-      <c r="F44" s="4"/>
+      <c r="A44" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B44" s="4">
+        <v>250000</v>
+      </c>
+      <c r="C44" s="4">
+        <f>SUM(I20:I25) * 12 + 4*I26</f>
+        <v>249900</v>
+      </c>
+      <c r="E44" s="4">
+        <f>B44-C44</f>
+        <v>100</v>
+      </c>
       <c r="G44" s="4"/>
-      <c r="H44" s="7"/>
+      <c r="H44" s="4"/>
       <c r="I44" s="4"/>
       <c r="J44" s="36"/>
       <c r="K44" s="3"/>
@@ -2370,18 +2354,17 @@
     </row>
     <row r="45" spans="1:21" ht="12.75" customHeight="1">
       <c r="A45" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B45" s="4">
         <v>250000</v>
       </c>
       <c r="C45" s="4">
-        <f>SUM(I20:I25) * 12 + 4*I26</f>
-        <v>249900</v>
+        <v>211176</v>
       </c>
       <c r="E45" s="4">
         <f>B45-C45</f>
-        <v>100</v>
+        <v>38824</v>
       </c>
       <c r="G45" s="4"/>
       <c r="H45" s="4"/>
@@ -2401,22 +2384,36 @@
     </row>
     <row r="46" spans="1:21" ht="12.75" customHeight="1">
       <c r="A46" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B46" s="4">
         <v>250000</v>
       </c>
       <c r="C46" s="4">
-        <v>211176</v>
-      </c>
+        <f>(29597 + 6488) + (3175 * 2 + 1258) + (3175 * 12) + (5354 * 3 + 1040) + (6075 + 10125 * 11) + (1331 + 3175 * 8)</f>
+        <v>243076</v>
+      </c>
+      <c r="D46" s="4"/>
       <c r="E46" s="4">
-        <f>B46-C46</f>
-        <v>38824</v>
-      </c>
-      <c r="G46" s="4"/>
-      <c r="H46" s="4"/>
-      <c r="I46" s="4"/>
-      <c r="J46" s="36"/>
+        <f t="shared" ref="E46:E48" si="0">B46-C46</f>
+        <v>6924</v>
+      </c>
+      <c r="F46" s="4"/>
+      <c r="G46">
+        <f>G40*0.1/12</f>
+        <v>0</v>
+      </c>
+      <c r="H46" s="17">
+        <v>9</v>
+      </c>
+      <c r="I46" s="17">
+        <f>G46*H46</f>
+        <v>0</v>
+      </c>
+      <c r="J46" s="35">
+        <f>C46+I46</f>
+        <v>243076</v>
+      </c>
       <c r="K46" s="3"/>
       <c r="L46" s="4"/>
       <c r="M46" s="4"/>
@@ -2431,19 +2428,19 @@
     </row>
     <row r="47" spans="1:21" ht="12.75" customHeight="1">
       <c r="A47" s="4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B47" s="4">
         <v>250000</v>
       </c>
       <c r="C47" s="4">
-        <f>(29597 + 6488) + (3175 * 2 + 1258) + (3175 * 12) + (5354 * 3 + 1040) + (6075 + 10125 * 11) + (1331 + 3175 * 8)</f>
-        <v>243076</v>
+        <f>(4030 * 3) + (3425 * 9) + (10215 * 12) + (4830 * 12) + 567 + (2309 * 9)</f>
+        <v>244803</v>
       </c>
       <c r="D47" s="4"/>
       <c r="E47" s="4">
-        <f t="shared" ref="E47:E49" si="0">B47-C47</f>
-        <v>6924</v>
+        <f>B47-C47</f>
+        <v>5197</v>
       </c>
       <c r="F47" s="4"/>
       <c r="G47">
@@ -2459,7 +2456,7 @@
       </c>
       <c r="J47" s="35">
         <f>C47+I47</f>
-        <v>243076</v>
+        <v>244803</v>
       </c>
       <c r="K47" s="3"/>
       <c r="L47" s="4"/>
@@ -2475,36 +2472,24 @@
     </row>
     <row r="48" spans="1:21" ht="12.75" customHeight="1">
       <c r="A48" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B48" s="4">
         <v>250000</v>
       </c>
       <c r="C48" s="4">
-        <f>(4030 * 3) + (3425 * 9) + (10215 * 12) + (4830 * 12) + 567 + (2309 * 9)</f>
-        <v>244803</v>
+        <v>174204</v>
       </c>
       <c r="D48" s="4"/>
       <c r="E48" s="4">
-        <f>B48-C48</f>
-        <v>5197</v>
+        <f t="shared" si="0"/>
+        <v>75796</v>
       </c>
       <c r="F48" s="4"/>
-      <c r="G48">
-        <f>G42*0.1/12</f>
-        <v>0</v>
-      </c>
-      <c r="H48" s="17">
-        <v>9</v>
-      </c>
-      <c r="I48" s="17">
-        <f>G48*H48</f>
-        <v>0</v>
-      </c>
-      <c r="J48" s="35">
-        <f>C48+I48</f>
-        <v>244803</v>
-      </c>
+      <c r="G48" s="4"/>
+      <c r="H48" s="4"/>
+      <c r="I48" s="4"/>
+      <c r="J48" s="36"/>
       <c r="K48" s="3"/>
       <c r="L48" s="4"/>
       <c r="M48" s="4"/>
@@ -2518,25 +2503,16 @@
       <c r="U48" s="4"/>
     </row>
     <row r="49" spans="1:21" ht="12.75" customHeight="1">
-      <c r="A49" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B49" s="4">
-        <v>250000</v>
-      </c>
-      <c r="C49" s="4">
-        <v>174204</v>
-      </c>
+      <c r="A49" s="4"/>
+      <c r="B49" s="4"/>
+      <c r="C49" s="4"/>
       <c r="D49" s="4"/>
-      <c r="E49" s="4">
-        <f t="shared" si="0"/>
-        <v>75796</v>
-      </c>
+      <c r="E49" s="4"/>
       <c r="F49" s="4"/>
       <c r="G49" s="4"/>
       <c r="H49" s="4"/>
       <c r="I49" s="4"/>
-      <c r="J49" s="36"/>
+      <c r="J49" s="3"/>
       <c r="K49" s="3"/>
       <c r="L49" s="4"/>
       <c r="M49" s="4"/>
@@ -2642,7 +2618,7 @@
       <c r="U53" s="4"/>
     </row>
     <row r="54" spans="1:21" ht="12.75" customHeight="1">
-      <c r="A54" s="4"/>
+      <c r="A54" s="35"/>
       <c r="B54" s="4"/>
       <c r="C54" s="4"/>
       <c r="D54" s="4"/>
@@ -2665,7 +2641,7 @@
       <c r="U54" s="4"/>
     </row>
     <row r="55" spans="1:21" ht="12.75" customHeight="1">
-      <c r="A55" s="35"/>
+      <c r="A55" s="4"/>
       <c r="B55" s="4"/>
       <c r="C55" s="4"/>
       <c r="D55" s="4"/>
@@ -3998,29 +3974,6 @@
       <c r="T112" s="4"/>
       <c r="U112" s="4"/>
     </row>
-    <row r="113" spans="1:21" ht="12.75" customHeight="1">
-      <c r="A113" s="4"/>
-      <c r="B113" s="4"/>
-      <c r="C113" s="4"/>
-      <c r="D113" s="4"/>
-      <c r="E113" s="4"/>
-      <c r="F113" s="4"/>
-      <c r="G113" s="4"/>
-      <c r="H113" s="4"/>
-      <c r="I113" s="4"/>
-      <c r="J113" s="3"/>
-      <c r="K113" s="3"/>
-      <c r="L113" s="4"/>
-      <c r="M113" s="4"/>
-      <c r="N113" s="4"/>
-      <c r="O113" s="4"/>
-      <c r="P113" s="4"/>
-      <c r="Q113" s="4"/>
-      <c r="R113" s="4"/>
-      <c r="S113" s="4"/>
-      <c r="T113" s="4"/>
-      <c r="U113" s="4"/>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" firstPageNumber="0" fitToWidth="0" fitToHeight="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>